<commit_message>
some progress on the srs script
</commit_message>
<xml_diff>
--- a/dikb-evidence/2017-evidence/cyp3a4-and-cyp2d6-substrates-2017-evidence-combined.xlsx
+++ b/dikb-evidence/2017-evidence/cyp3a4-and-cyp2d6-substrates-2017-evidence-combined.xlsx
@@ -16,6 +16,8 @@
     <sheet name="Sheet1" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'cyp2d6-or-cyp3a4-increase-auc-e'!$A$1:$H$56</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'cyp2d6-or-cyp3a4-inhibitors-dik'!$A$1:$G$182</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'cyp2d6-or-cyp3a4-substrates-dik'!$A$1:$G$121</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">DDIPredictions_Lax_2017_evidenc!$A$1:$E$933</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">DDIPredictions_Strict_2017_evid!$A$1:$E$306</definedName>
@@ -1918,6 +1920,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="true">
@@ -25891,16 +25901,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G182"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.96"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -25925,7 +25938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>274</v>
       </c>
@@ -25948,7 +25961,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>253</v>
       </c>
@@ -25971,7 +25984,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>24</v>
       </c>
@@ -25994,7 +26007,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>328</v>
       </c>
@@ -26040,7 +26053,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>331</v>
       </c>
@@ -26063,7 +26076,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>89</v>
       </c>
@@ -26086,7 +26099,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>254</v>
       </c>
@@ -26109,7 +26122,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>335</v>
       </c>
@@ -26132,7 +26145,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>263</v>
       </c>
@@ -26155,7 +26168,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>198</v>
       </c>
@@ -26178,7 +26191,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>265</v>
       </c>
@@ -26201,7 +26214,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>280</v>
       </c>
@@ -26224,7 +26237,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>277</v>
       </c>
@@ -26247,7 +26260,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>183</v>
       </c>
@@ -26270,7 +26283,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>183</v>
       </c>
@@ -26293,7 +26306,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>183</v>
       </c>
@@ -26316,7 +26329,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>293</v>
       </c>
@@ -26339,7 +26352,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>293</v>
       </c>
@@ -26362,7 +26375,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>293</v>
       </c>
@@ -26385,7 +26398,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>71</v>
       </c>
@@ -26408,7 +26421,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>200</v>
       </c>
@@ -26431,7 +26444,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>62</v>
       </c>
@@ -26454,7 +26467,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>278</v>
       </c>
@@ -26477,7 +26490,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>271</v>
       </c>
@@ -26500,7 +26513,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>271</v>
       </c>
@@ -26523,7 +26536,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>271</v>
       </c>
@@ -26546,7 +26559,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>271</v>
       </c>
@@ -26569,7 +26582,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>283</v>
       </c>
@@ -26592,7 +26605,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>53</v>
       </c>
@@ -26615,7 +26628,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>53</v>
       </c>
@@ -26638,7 +26651,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>116</v>
       </c>
@@ -26661,7 +26674,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>50</v>
       </c>
@@ -26684,7 +26697,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>363</v>
       </c>
@@ -26707,7 +26720,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>319</v>
       </c>
@@ -26730,7 +26743,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>319</v>
       </c>
@@ -26753,7 +26766,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>319</v>
       </c>
@@ -26776,7 +26789,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>220</v>
       </c>
@@ -26799,7 +26812,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>140</v>
       </c>
@@ -26822,7 +26835,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>81</v>
       </c>
@@ -26845,7 +26858,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>371</v>
       </c>
@@ -26868,7 +26881,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>262</v>
       </c>
@@ -26891,7 +26904,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>262</v>
       </c>
@@ -26914,7 +26927,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>262</v>
       </c>
@@ -26937,7 +26950,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>261</v>
       </c>
@@ -26960,7 +26973,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>261</v>
       </c>
@@ -26983,7 +26996,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>261</v>
       </c>
@@ -27006,7 +27019,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>261</v>
       </c>
@@ -27029,7 +27042,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>261</v>
       </c>
@@ -27052,7 +27065,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>261</v>
       </c>
@@ -27075,7 +27088,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>313</v>
       </c>
@@ -27098,7 +27111,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>245</v>
       </c>
@@ -27121,7 +27134,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>244</v>
       </c>
@@ -27144,7 +27157,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>384</v>
       </c>
@@ -27167,7 +27180,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>29</v>
       </c>
@@ -27190,7 +27203,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>29</v>
       </c>
@@ -27213,7 +27226,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>29</v>
       </c>
@@ -27236,7 +27249,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>218</v>
       </c>
@@ -27259,7 +27272,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>218</v>
       </c>
@@ -27282,7 +27295,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>247</v>
       </c>
@@ -27305,7 +27318,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>247</v>
       </c>
@@ -27328,7 +27341,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>35</v>
       </c>
@@ -27374,7 +27387,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>35</v>
       </c>
@@ -27397,7 +27410,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>284</v>
       </c>
@@ -27420,7 +27433,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>282</v>
       </c>
@@ -27466,7 +27479,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>254</v>
       </c>
@@ -27489,7 +27502,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>85</v>
       </c>
@@ -27512,7 +27525,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>85</v>
       </c>
@@ -27535,7 +27548,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>85</v>
       </c>
@@ -27558,7 +27571,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>268</v>
       </c>
@@ -27581,7 +27594,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>295</v>
       </c>
@@ -27604,7 +27617,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>295</v>
       </c>
@@ -27627,7 +27640,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>127</v>
       </c>
@@ -27650,7 +27663,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>238</v>
       </c>
@@ -27673,7 +27686,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>247</v>
       </c>
@@ -27696,7 +27709,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>247</v>
       </c>
@@ -27742,7 +27755,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>260</v>
       </c>
@@ -27765,7 +27778,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>260</v>
       </c>
@@ -27788,7 +27801,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>148</v>
       </c>
@@ -27811,7 +27824,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>66</v>
       </c>
@@ -27834,7 +27847,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>66</v>
       </c>
@@ -27857,7 +27870,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>66</v>
       </c>
@@ -27880,7 +27893,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>66</v>
       </c>
@@ -27903,7 +27916,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>241</v>
       </c>
@@ -27926,7 +27939,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>241</v>
       </c>
@@ -27949,7 +27962,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>415</v>
       </c>
@@ -27972,7 +27985,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>296</v>
       </c>
@@ -27995,7 +28008,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>291</v>
       </c>
@@ -28018,7 +28031,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>281</v>
       </c>
@@ -28041,7 +28054,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>252</v>
       </c>
@@ -28064,7 +28077,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>421</v>
       </c>
@@ -28087,7 +28100,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>96</v>
       </c>
@@ -28110,7 +28123,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>273</v>
       </c>
@@ -28156,7 +28169,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>218</v>
       </c>
@@ -28179,7 +28192,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>311</v>
       </c>
@@ -28202,7 +28215,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>264</v>
       </c>
@@ -28225,7 +28238,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>264</v>
       </c>
@@ -28248,7 +28261,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>264</v>
       </c>
@@ -28317,7 +28330,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>269</v>
       </c>
@@ -28340,7 +28353,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>269</v>
       </c>
@@ -28363,7 +28376,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>269</v>
       </c>
@@ -28386,7 +28399,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>286</v>
       </c>
@@ -28409,7 +28422,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>286</v>
       </c>
@@ -28432,7 +28445,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>286</v>
       </c>
@@ -28455,7 +28468,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>214</v>
       </c>
@@ -28478,7 +28491,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>265</v>
       </c>
@@ -28501,7 +28514,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>304</v>
       </c>
@@ -28524,7 +28537,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>234</v>
       </c>
@@ -28547,7 +28560,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>105</v>
       </c>
@@ -28570,7 +28583,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>62</v>
       </c>
@@ -28593,7 +28606,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>62</v>
       </c>
@@ -28616,7 +28629,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>18</v>
       </c>
@@ -28639,7 +28652,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>18</v>
       </c>
@@ -28662,7 +28675,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>303</v>
       </c>
@@ -28685,7 +28698,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>278</v>
       </c>
@@ -28708,7 +28721,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>278</v>
       </c>
@@ -28731,7 +28744,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>241</v>
       </c>
@@ -28754,7 +28767,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>244</v>
       </c>
@@ -28777,7 +28790,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>244</v>
       </c>
@@ -28800,7 +28813,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>244</v>
       </c>
@@ -28823,7 +28836,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>7</v>
       </c>
@@ -28846,7 +28859,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>85</v>
       </c>
@@ -28869,7 +28882,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>257</v>
       </c>
@@ -28892,7 +28905,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>425</v>
       </c>
@@ -28915,7 +28928,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>299</v>
       </c>
@@ -28938,7 +28951,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>29</v>
       </c>
@@ -28961,7 +28974,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>459</v>
       </c>
@@ -28984,7 +28997,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>461</v>
       </c>
@@ -29007,7 +29020,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>305</v>
       </c>
@@ -29076,7 +29089,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>307</v>
       </c>
@@ -29099,7 +29112,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>53</v>
       </c>
@@ -29122,7 +29135,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>53</v>
       </c>
@@ -29145,7 +29158,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>53</v>
       </c>
@@ -29168,7 +29181,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>53</v>
       </c>
@@ -29191,7 +29204,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>285</v>
       </c>
@@ -29237,7 +29250,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>252</v>
       </c>
@@ -29260,7 +29273,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>195</v>
       </c>
@@ -29283,7 +29296,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>195</v>
       </c>
@@ -29306,7 +29319,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>195</v>
       </c>
@@ -29352,7 +29365,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>136</v>
       </c>
@@ -29375,7 +29388,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>136</v>
       </c>
@@ -29398,7 +29411,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>136</v>
       </c>
@@ -29421,7 +29434,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>136</v>
       </c>
@@ -29444,7 +29457,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>136</v>
       </c>
@@ -29467,7 +29480,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>136</v>
       </c>
@@ -29490,7 +29503,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>384</v>
       </c>
@@ -29513,7 +29526,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>384</v>
       </c>
@@ -29536,7 +29549,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>384</v>
       </c>
@@ -29559,7 +29572,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>207</v>
       </c>
@@ -29582,7 +29595,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>207</v>
       </c>
@@ -29605,7 +29618,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>207</v>
       </c>
@@ -29628,7 +29641,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>207</v>
       </c>
@@ -29651,7 +29664,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>177</v>
       </c>
@@ -29674,7 +29687,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>177</v>
       </c>
@@ -29697,7 +29710,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>177</v>
       </c>
@@ -29720,7 +29733,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>177</v>
       </c>
@@ -29743,7 +29756,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
         <v>66</v>
       </c>
@@ -29766,7 +29779,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
         <v>132</v>
       </c>
@@ -29789,7 +29802,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
         <v>256</v>
       </c>
@@ -29812,7 +29825,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>220</v>
       </c>
@@ -29835,7 +29848,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>396</v>
       </c>
@@ -29858,7 +29871,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
         <v>396</v>
       </c>
@@ -29881,7 +29894,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
         <v>276</v>
       </c>
@@ -29904,7 +29917,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>276</v>
       </c>
@@ -29973,7 +29986,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>89</v>
       </c>
@@ -29996,7 +30009,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>89</v>
       </c>
@@ -30019,7 +30032,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>89</v>
       </c>
@@ -30042,7 +30055,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
         <v>286</v>
       </c>
@@ -30065,7 +30078,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
         <v>286</v>
       </c>
@@ -30089,6 +30102,23 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G182">
+    <filterColumn colId="2">
+      <customFilters and="true">
+        <customFilter operator="equal" val="cyp2d6"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <customFilters and="true">
+        <customFilter operator="equal" val="EVIDENCE AGAINST"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Non_traceable_Drug_Label_Statement"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -30096,49 +30126,50 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>295</v>
       </c>
@@ -30164,7 +30195,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>207</v>
       </c>
@@ -30190,7 +30221,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>136</v>
       </c>
@@ -30216,7 +30247,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>278</v>
       </c>
@@ -30242,7 +30273,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>271</v>
       </c>
@@ -30268,7 +30299,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>262</v>
       </c>
@@ -30294,7 +30325,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>271</v>
       </c>
@@ -30346,7 +30377,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>218</v>
       </c>
@@ -30372,7 +30403,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>177</v>
       </c>
@@ -30398,7 +30429,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>269</v>
       </c>
@@ -30450,7 +30481,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>278</v>
       </c>
@@ -30476,7 +30507,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>271</v>
       </c>
@@ -30554,7 +30585,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>207</v>
       </c>
@@ -30580,7 +30611,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>136</v>
       </c>
@@ -30606,7 +30637,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>261</v>
       </c>
@@ -30632,7 +30663,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>207</v>
       </c>
@@ -30658,7 +30689,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>207</v>
       </c>
@@ -30684,7 +30715,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>207</v>
       </c>
@@ -30710,7 +30741,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>262</v>
       </c>
@@ -30736,7 +30767,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>271</v>
       </c>
@@ -30866,7 +30897,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>261</v>
       </c>
@@ -30892,7 +30923,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>261</v>
       </c>
@@ -30918,7 +30949,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>177</v>
       </c>
@@ -30970,7 +31001,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>177</v>
       </c>
@@ -30996,7 +31027,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>177</v>
       </c>
@@ -31022,7 +31053,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>261</v>
       </c>
@@ -31048,7 +31079,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>247</v>
       </c>
@@ -31100,7 +31131,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>262</v>
       </c>
@@ -31126,7 +31157,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>262</v>
       </c>
@@ -31152,7 +31183,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>269</v>
       </c>
@@ -31178,7 +31209,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>269</v>
       </c>
@@ -31204,7 +31235,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>269</v>
       </c>
@@ -31230,7 +31261,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>311</v>
       </c>
@@ -31308,7 +31339,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>295</v>
       </c>
@@ -31360,7 +31391,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>261</v>
       </c>
@@ -31386,7 +31417,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>262</v>
       </c>
@@ -31412,7 +31443,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>262</v>
       </c>
@@ -31438,7 +31469,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>293</v>
       </c>
@@ -31464,7 +31495,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>136</v>
       </c>
@@ -31490,7 +31521,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>136</v>
       </c>
@@ -31516,7 +31547,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>136</v>
       </c>
@@ -31542,7 +31573,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>271</v>
       </c>
@@ -31569,6 +31600,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H56">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="diltiazem"/>
+        <filter val="fluoxetine"/>
+        <filter val="fluvoxamine"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -31576,6 +31616,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
showing owl semantics for 7-OH-mitrag
</commit_message>
<xml_diff>
--- a/dikb-evidence/2017-evidence/cyp3a4-and-cyp2d6-substrates-2017-evidence-combined.xlsx
+++ b/dikb-evidence/2017-evidence/cyp3a4-and-cyp2d6-substrates-2017-evidence-combined.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="cyp2d6-or-cyp3a4-substrates-dik" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,10 +17,10 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'cyp2d6-or-cyp3a4-increase-auc-e'!$A$1:$H$56</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'cyp2d6-or-cyp3a4-inhibitors-dik'!$A$1:$G$182</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'cyp2d6-or-cyp3a4-substrates-dik'!$A$1:$G$121</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">DDIPredictions_Lax_2017_evidenc!$A$1:$E$933</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">DDIPredictions_Strict_2017_evid!$A$1:$E$306</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'cyp2d6-or-cyp3a4-inhibitors-dik'!$A$1:$G$182</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -1828,6 +1828,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1924,10 +1925,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="true">
@@ -1935,11 +1932,11 @@
   </sheetPr>
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.76"/>
@@ -2084,7 +2081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>18</v>
       </c>
@@ -2130,7 +2127,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -2245,7 +2242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>38</v>
       </c>
@@ -2268,7 +2265,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>38</v>
       </c>
@@ -2291,7 +2288,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>41</v>
       </c>
@@ -2314,7 +2311,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>41</v>
       </c>
@@ -2360,7 +2357,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>46</v>
       </c>
@@ -2429,7 +2426,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>53</v>
       </c>
@@ -2452,7 +2449,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>53</v>
       </c>
@@ -2475,7 +2472,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>56</v>
       </c>
@@ -2636,7 +2633,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>71</v>
       </c>
@@ -2682,7 +2679,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>75</v>
       </c>
@@ -2705,7 +2702,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>78</v>
       </c>
@@ -2728,7 +2725,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>81</v>
       </c>
@@ -2935,7 +2932,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>98</v>
       </c>
@@ -2958,7 +2955,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>100</v>
       </c>
@@ -2981,7 +2978,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>103</v>
       </c>
@@ -3027,7 +3024,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>108</v>
       </c>
@@ -3050,7 +3047,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>111</v>
       </c>
@@ -3188,7 +3185,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>121</v>
       </c>
@@ -3211,7 +3208,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>121</v>
       </c>
@@ -3234,7 +3231,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>124</v>
       </c>
@@ -3257,7 +3254,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>127</v>
       </c>
@@ -3441,7 +3438,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>146</v>
       </c>
@@ -3464,7 +3461,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>148</v>
       </c>
@@ -3487,7 +3484,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>150</v>
       </c>
@@ -3602,7 +3599,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>160</v>
       </c>
@@ -3671,7 +3668,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>50</v>
       </c>
@@ -3901,7 +3898,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>75</v>
       </c>
@@ -4016,7 +4013,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>157</v>
       </c>
@@ -4108,7 +4105,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>87</v>
       </c>
@@ -4223,7 +4220,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>195</v>
       </c>
@@ -4246,7 +4243,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>198</v>
       </c>
@@ -4269,7 +4266,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>200</v>
       </c>
@@ -4430,7 +4427,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>211</v>
       </c>
@@ -4522,7 +4519,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>218</v>
       </c>
@@ -4545,7 +4542,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>220</v>
       </c>
@@ -4591,7 +4588,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>140</v>
       </c>
@@ -4733,18 +4730,19 @@
   <autoFilter ref="A1:G121">
     <filterColumn colId="2">
       <customFilters and="true">
-        <customFilter operator="equal" val="cyp2d6"/>
+        <customFilter operator="equal" val="cyp3a4"/>
       </customFilters>
     </filterColumn>
     <filterColumn colId="3">
       <customFilters and="true">
-        <customFilter operator="equal" val="EVIDENCE AGAINST"/>
+        <customFilter operator="equal" val="EVIDENCE FOR"/>
       </customFilters>
     </filterColumn>
     <filterColumn colId="5">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Non_traceable_Drug_Label_Statement"/>
-      </customFilters>
+      <filters>
+        <filter val="Non_Tracable_Statement"/>
+        <filter val="Non_traceable_Drug_Label_Statement"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4769,12 +4767,12 @@
       <selection pane="topLeft" activeCell="I612" activeCellId="0" sqref="I612"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.94"/>
   </cols>
   <sheetData>
@@ -20649,7 +20647,7 @@
   </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -20669,12 +20667,12 @@
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.94"/>
   </cols>
   <sheetData>
@@ -25890,7 +25888,7 @@
   </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -25901,16 +25899,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G182"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.96"/>
   </cols>
@@ -25938,7 +25936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>274</v>
       </c>
@@ -25961,7 +25959,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>253</v>
       </c>
@@ -25984,7 +25982,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>24</v>
       </c>
@@ -26007,7 +26005,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>328</v>
       </c>
@@ -26053,7 +26051,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>331</v>
       </c>
@@ -26076,7 +26074,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>89</v>
       </c>
@@ -26099,7 +26097,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>254</v>
       </c>
@@ -26122,7 +26120,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>335</v>
       </c>
@@ -26145,7 +26143,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>263</v>
       </c>
@@ -26168,7 +26166,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>198</v>
       </c>
@@ -26191,7 +26189,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>265</v>
       </c>
@@ -26214,7 +26212,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>280</v>
       </c>
@@ -26237,7 +26235,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>277</v>
       </c>
@@ -26260,7 +26258,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>183</v>
       </c>
@@ -26283,7 +26281,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>183</v>
       </c>
@@ -26306,7 +26304,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>183</v>
       </c>
@@ -26329,7 +26327,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>293</v>
       </c>
@@ -26352,7 +26350,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>293</v>
       </c>
@@ -26375,7 +26373,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>293</v>
       </c>
@@ -26398,7 +26396,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>71</v>
       </c>
@@ -26421,7 +26419,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>200</v>
       </c>
@@ -26444,7 +26442,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>62</v>
       </c>
@@ -26467,7 +26465,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>278</v>
       </c>
@@ -26490,7 +26488,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>271</v>
       </c>
@@ -26513,7 +26511,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>271</v>
       </c>
@@ -26536,7 +26534,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>271</v>
       </c>
@@ -26559,7 +26557,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>271</v>
       </c>
@@ -26582,7 +26580,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>283</v>
       </c>
@@ -26605,7 +26603,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>53</v>
       </c>
@@ -26628,7 +26626,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>53</v>
       </c>
@@ -26651,7 +26649,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>116</v>
       </c>
@@ -26674,7 +26672,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>50</v>
       </c>
@@ -26697,7 +26695,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>363</v>
       </c>
@@ -26720,7 +26718,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>319</v>
       </c>
@@ -26743,7 +26741,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>319</v>
       </c>
@@ -26766,7 +26764,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>319</v>
       </c>
@@ -26789,7 +26787,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>220</v>
       </c>
@@ -26812,7 +26810,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>140</v>
       </c>
@@ -26835,7 +26833,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>81</v>
       </c>
@@ -26858,7 +26856,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>371</v>
       </c>
@@ -26881,7 +26879,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>262</v>
       </c>
@@ -26904,7 +26902,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>262</v>
       </c>
@@ -26927,7 +26925,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>262</v>
       </c>
@@ -26950,7 +26948,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>261</v>
       </c>
@@ -26973,7 +26971,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>261</v>
       </c>
@@ -26996,7 +26994,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>261</v>
       </c>
@@ -27019,7 +27017,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>261</v>
       </c>
@@ -27042,7 +27040,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>261</v>
       </c>
@@ -27065,7 +27063,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>261</v>
       </c>
@@ -27088,7 +27086,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>313</v>
       </c>
@@ -27111,7 +27109,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>245</v>
       </c>
@@ -27134,7 +27132,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>244</v>
       </c>
@@ -27157,7 +27155,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>384</v>
       </c>
@@ -27180,7 +27178,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>29</v>
       </c>
@@ -27203,7 +27201,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>29</v>
       </c>
@@ -27226,7 +27224,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>29</v>
       </c>
@@ -27249,7 +27247,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>218</v>
       </c>
@@ -27272,7 +27270,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>218</v>
       </c>
@@ -27295,7 +27293,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>247</v>
       </c>
@@ -27318,7 +27316,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>247</v>
       </c>
@@ -27341,7 +27339,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>35</v>
       </c>
@@ -27387,7 +27385,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>35</v>
       </c>
@@ -27410,7 +27408,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>284</v>
       </c>
@@ -27433,7 +27431,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>282</v>
       </c>
@@ -27479,7 +27477,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>254</v>
       </c>
@@ -27502,7 +27500,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>85</v>
       </c>
@@ -27525,7 +27523,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>85</v>
       </c>
@@ -27548,7 +27546,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>85</v>
       </c>
@@ -27571,7 +27569,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>268</v>
       </c>
@@ -27594,7 +27592,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>295</v>
       </c>
@@ -27617,7 +27615,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>295</v>
       </c>
@@ -27640,7 +27638,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>127</v>
       </c>
@@ -27663,7 +27661,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>238</v>
       </c>
@@ -27686,7 +27684,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>247</v>
       </c>
@@ -27709,7 +27707,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>247</v>
       </c>
@@ -27755,7 +27753,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>260</v>
       </c>
@@ -27778,7 +27776,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>260</v>
       </c>
@@ -27801,7 +27799,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>148</v>
       </c>
@@ -27824,7 +27822,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>66</v>
       </c>
@@ -27847,7 +27845,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>66</v>
       </c>
@@ -27870,7 +27868,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>66</v>
       </c>
@@ -27893,7 +27891,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>66</v>
       </c>
@@ -27916,7 +27914,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>241</v>
       </c>
@@ -27939,7 +27937,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>241</v>
       </c>
@@ -27962,7 +27960,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>415</v>
       </c>
@@ -27985,7 +27983,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>296</v>
       </c>
@@ -28008,7 +28006,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>291</v>
       </c>
@@ -28031,7 +28029,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>281</v>
       </c>
@@ -28054,7 +28052,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>252</v>
       </c>
@@ -28077,7 +28075,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>421</v>
       </c>
@@ -28100,7 +28098,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>96</v>
       </c>
@@ -28123,7 +28121,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>273</v>
       </c>
@@ -28169,7 +28167,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>218</v>
       </c>
@@ -28192,7 +28190,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>311</v>
       </c>
@@ -28215,7 +28213,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>264</v>
       </c>
@@ -28238,7 +28236,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>264</v>
       </c>
@@ -28261,7 +28259,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>264</v>
       </c>
@@ -28330,7 +28328,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>269</v>
       </c>
@@ -28353,7 +28351,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>269</v>
       </c>
@@ -28376,7 +28374,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>269</v>
       </c>
@@ -28399,7 +28397,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>286</v>
       </c>
@@ -28422,7 +28420,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>286</v>
       </c>
@@ -28445,7 +28443,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>286</v>
       </c>
@@ -28468,7 +28466,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>214</v>
       </c>
@@ -28491,7 +28489,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>265</v>
       </c>
@@ -28514,7 +28512,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>304</v>
       </c>
@@ -28537,7 +28535,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>234</v>
       </c>
@@ -28560,7 +28558,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>105</v>
       </c>
@@ -28583,7 +28581,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>62</v>
       </c>
@@ -28606,7 +28604,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>62</v>
       </c>
@@ -28629,7 +28627,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>18</v>
       </c>
@@ -28652,7 +28650,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>18</v>
       </c>
@@ -28675,7 +28673,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>303</v>
       </c>
@@ -28698,7 +28696,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>278</v>
       </c>
@@ -28721,7 +28719,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>278</v>
       </c>
@@ -28744,7 +28742,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>241</v>
       </c>
@@ -28767,7 +28765,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>244</v>
       </c>
@@ -28790,7 +28788,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>244</v>
       </c>
@@ -28813,7 +28811,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>244</v>
       </c>
@@ -28836,7 +28834,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>7</v>
       </c>
@@ -28859,7 +28857,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>85</v>
       </c>
@@ -28882,7 +28880,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>257</v>
       </c>
@@ -28905,7 +28903,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>425</v>
       </c>
@@ -28928,7 +28926,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>299</v>
       </c>
@@ -28951,7 +28949,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>29</v>
       </c>
@@ -28974,7 +28972,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>459</v>
       </c>
@@ -28997,7 +28995,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>461</v>
       </c>
@@ -29020,7 +29018,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>305</v>
       </c>
@@ -29089,7 +29087,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>307</v>
       </c>
@@ -29112,7 +29110,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>53</v>
       </c>
@@ -29135,7 +29133,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>53</v>
       </c>
@@ -29158,7 +29156,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>53</v>
       </c>
@@ -29181,7 +29179,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>53</v>
       </c>
@@ -29204,7 +29202,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>285</v>
       </c>
@@ -29250,7 +29248,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>252</v>
       </c>
@@ -29273,7 +29271,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>195</v>
       </c>
@@ -29296,7 +29294,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>195</v>
       </c>
@@ -29319,7 +29317,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>195</v>
       </c>
@@ -29365,7 +29363,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>136</v>
       </c>
@@ -29388,7 +29386,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>136</v>
       </c>
@@ -29411,7 +29409,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>136</v>
       </c>
@@ -29434,7 +29432,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>136</v>
       </c>
@@ -29457,7 +29455,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>136</v>
       </c>
@@ -29480,7 +29478,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>136</v>
       </c>
@@ -29503,7 +29501,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>384</v>
       </c>
@@ -29526,7 +29524,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>384</v>
       </c>
@@ -29549,7 +29547,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>384</v>
       </c>
@@ -29572,7 +29570,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>207</v>
       </c>
@@ -29595,7 +29593,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>207</v>
       </c>
@@ -29618,7 +29616,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>207</v>
       </c>
@@ -29641,7 +29639,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>207</v>
       </c>
@@ -29664,7 +29662,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>177</v>
       </c>
@@ -29687,7 +29685,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>177</v>
       </c>
@@ -29710,7 +29708,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>177</v>
       </c>
@@ -29733,7 +29731,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>177</v>
       </c>
@@ -29756,7 +29754,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
         <v>66</v>
       </c>
@@ -29779,7 +29777,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
         <v>132</v>
       </c>
@@ -29802,7 +29800,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
         <v>256</v>
       </c>
@@ -29825,7 +29823,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>220</v>
       </c>
@@ -29848,7 +29846,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>396</v>
       </c>
@@ -29871,7 +29869,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
         <v>396</v>
       </c>
@@ -29894,7 +29892,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
         <v>276</v>
       </c>
@@ -29917,7 +29915,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>276</v>
       </c>
@@ -29986,7 +29984,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>89</v>
       </c>
@@ -30009,7 +30007,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>89</v>
       </c>
@@ -30032,7 +30030,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>89</v>
       </c>
@@ -30055,7 +30053,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
         <v>286</v>
       </c>
@@ -30078,7 +30076,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
         <v>286</v>
       </c>
@@ -30102,46 +30100,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G182">
-    <filterColumn colId="2">
-      <customFilters and="true">
-        <customFilter operator="equal" val="cyp2d6"/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <customFilters and="true">
-        <customFilter operator="equal" val="EVIDENCE AGAINST"/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Non_traceable_Drug_Label_Statement"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -30169,7 +30149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>295</v>
       </c>
@@ -30195,7 +30175,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>207</v>
       </c>
@@ -30221,7 +30201,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>136</v>
       </c>
@@ -30247,7 +30227,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>278</v>
       </c>
@@ -30273,7 +30253,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>271</v>
       </c>
@@ -30299,7 +30279,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>262</v>
       </c>
@@ -30325,7 +30305,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>271</v>
       </c>
@@ -30377,7 +30357,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>218</v>
       </c>
@@ -30403,7 +30383,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>177</v>
       </c>
@@ -30429,7 +30409,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>269</v>
       </c>
@@ -30481,7 +30461,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>278</v>
       </c>
@@ -30507,7 +30487,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>271</v>
       </c>
@@ -30585,7 +30565,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>207</v>
       </c>
@@ -30611,7 +30591,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>136</v>
       </c>
@@ -30637,7 +30617,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>261</v>
       </c>
@@ -30663,7 +30643,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>207</v>
       </c>
@@ -30689,7 +30669,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>207</v>
       </c>
@@ -30715,7 +30695,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>207</v>
       </c>
@@ -30741,7 +30721,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>262</v>
       </c>
@@ -30767,7 +30747,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>271</v>
       </c>
@@ -30897,7 +30877,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>261</v>
       </c>
@@ -30923,7 +30903,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>261</v>
       </c>
@@ -30949,7 +30929,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>177</v>
       </c>
@@ -31001,7 +30981,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>177</v>
       </c>
@@ -31027,7 +31007,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>177</v>
       </c>
@@ -31053,7 +31033,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>261</v>
       </c>
@@ -31079,7 +31059,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>247</v>
       </c>
@@ -31131,7 +31111,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>262</v>
       </c>
@@ -31157,7 +31137,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>262</v>
       </c>
@@ -31183,7 +31163,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>269</v>
       </c>
@@ -31209,7 +31189,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>269</v>
       </c>
@@ -31235,7 +31215,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>269</v>
       </c>
@@ -31261,7 +31241,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>311</v>
       </c>
@@ -31339,7 +31319,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>295</v>
       </c>
@@ -31391,7 +31371,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>261</v>
       </c>
@@ -31417,7 +31397,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>262</v>
       </c>
@@ -31443,7 +31423,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>262</v>
       </c>
@@ -31469,7 +31449,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>293</v>
       </c>
@@ -31495,7 +31475,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>136</v>
       </c>
@@ -31521,7 +31501,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>136</v>
       </c>
@@ -31547,7 +31527,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>136</v>
       </c>
@@ -31573,7 +31553,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>271</v>
       </c>
@@ -31600,18 +31580,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H56">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="diltiazem"/>
-        <filter val="fluoxetine"/>
-        <filter val="fluvoxamine"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H56"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -31631,11 +31603,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>